<commit_message>
add table to min max
</commit_message>
<xml_diff>
--- a/lab.xlsx
+++ b/lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teknikkomputer/Documents/node/labexcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1B82D6-C873-224E-B93A-23748B176B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399678D2-4A0A-E642-86B7-E1205EAD7722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1238,6 +1238,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1256,8 +1262,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4988,13 +4997,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -5469,11 +5478,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -5529,13 +5538,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -5847,11 +5856,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -5906,13 +5915,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6190,11 +6199,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6249,13 +6258,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6525,11 +6534,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6584,13 +6593,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6859,11 +6868,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6919,13 +6928,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7226,11 +7235,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -7285,13 +7294,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7524,11 +7533,11 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="69" t="s">
+      <c r="B36" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
       <c r="E36" s="3" t="s">
         <v>72</v>
       </c>
@@ -7583,13 +7592,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7872,11 +7881,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -7931,13 +7940,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8232,11 +8241,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -8291,13 +8300,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8654,11 +8663,11 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
       <c r="E45" s="3" t="s">
         <v>72</v>
       </c>
@@ -8708,13 +8717,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8793,12 +8802,12 @@
       <c r="A18" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="45"/>
       <c r="G18" s="26"/>
     </row>
@@ -8806,40 +8815,40 @@
       <c r="A19" s="61" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
         <v>255</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
       <c r="F22" s="2"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -8995,11 +9004,11 @@
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="69" t="s">
+      <c r="B43" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
       <c r="E43" s="3" t="s">
         <v>72</v>
       </c>
@@ -9029,7 +9038,7 @@
   <dimension ref="A6:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9054,13 +9063,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -9135,25 +9144,25 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="76" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9165,7 +9174,8 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
@@ -9176,10 +9186,11 @@
       <c r="D20" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
@@ -9187,13 +9198,14 @@
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
@@ -9201,13 +9213,14 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
@@ -9215,16 +9228,16 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="68">
         <v>4</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="12">
         <v>6</v>
       </c>
     </row>
@@ -9234,16 +9247,16 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="12"/>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="68">
         <v>1</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="12">
         <v>3</v>
       </c>
     </row>
@@ -9253,16 +9266,16 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="68">
         <v>0</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="12">
         <v>1</v>
       </c>
     </row>
@@ -9272,16 +9285,16 @@
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="68">
         <v>50</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="12">
         <v>70</v>
       </c>
     </row>
@@ -9291,16 +9304,16 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="12"/>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="68">
         <v>25</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="12">
         <v>35</v>
       </c>
     </row>
@@ -9313,13 +9326,13 @@
       <c r="D28" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="68">
         <v>4</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="12">
         <v>6</v>
       </c>
     </row>
@@ -9332,13 +9345,13 @@
       <c r="D29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="68">
         <v>1</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="12">
         <v>2</v>
       </c>
     </row>
@@ -9351,13 +9364,13 @@
       <c r="D30" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="68">
         <v>0</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="12">
         <v>1</v>
       </c>
     </row>
@@ -9370,13 +9383,13 @@
       <c r="D31" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="68">
         <v>3900000</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="12">
         <v>4800000</v>
       </c>
     </row>
@@ -9389,13 +9402,13 @@
       <c r="D32" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="73">
+      <c r="F32" s="75">
         <v>11.4</v>
       </c>
-      <c r="G32" s="73">
+      <c r="G32" s="75">
         <v>15.1</v>
       </c>
     </row>
@@ -9408,13 +9421,13 @@
       <c r="D33" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="68">
         <v>40</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="12">
         <v>42</v>
       </c>
     </row>
@@ -9424,16 +9437,16 @@
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="12"/>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="68">
         <v>80</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="12">
         <v>100</v>
       </c>
     </row>
@@ -9446,13 +9459,13 @@
       <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="68">
         <v>26</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="12">
         <v>34</v>
       </c>
     </row>
@@ -9462,16 +9475,16 @@
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="12"/>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="68">
         <v>31</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="12">
         <v>35</v>
       </c>
     </row>
@@ -9484,13 +9497,13 @@
       <c r="D37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="68">
         <v>10</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="12">
         <v>16</v>
       </c>
     </row>
@@ -9500,16 +9513,16 @@
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="12"/>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="68">
         <v>37</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="12">
         <v>46</v>
       </c>
     </row>
@@ -9519,16 +9532,16 @@
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="12"/>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="68">
         <v>150000</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="12">
         <v>400000</v>
       </c>
     </row>
@@ -9541,13 +9554,13 @@
       <c r="D40" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="68">
         <v>7</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="12">
         <v>11</v>
       </c>
     </row>
@@ -9560,13 +9573,13 @@
       <c r="D41" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="68">
         <v>10</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="12">
         <v>18</v>
       </c>
     </row>
@@ -9576,16 +9589,16 @@
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="12"/>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="73">
+      <c r="F42" s="75">
         <v>0.2</v>
       </c>
-      <c r="G42" s="73">
+      <c r="G42" s="75">
         <v>0.5</v>
       </c>
     </row>
@@ -9596,10 +9609,11 @@
       <c r="B43" s="14"/>
       <c r="C43" s="12"/>
       <c r="D43" s="14"/>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E44" s="8"/>
@@ -9639,11 +9653,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -9771,13 +9785,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -10252,11 +10266,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -10311,13 +10325,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -10792,11 +10806,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -10851,13 +10865,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -11234,11 +11248,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -11288,13 +11302,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -11671,11 +11685,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -11725,13 +11739,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -12108,11 +12122,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -12162,13 +12176,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -12545,11 +12559,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -12599,13 +12613,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -13018,11 +13032,11 @@
       <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
       <c r="E48" s="3" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
add data min max
</commit_message>
<xml_diff>
--- a/lab.xlsx
+++ b/lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teknikkomputer/Documents/node/labexcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399678D2-4A0A-E642-86B7-E1205EAD7722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FEFED0-66EB-B743-9642-0E7845277041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DL Laki - laki dewasa" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="269">
   <si>
     <t xml:space="preserve">Laporan Hasil Pemeriksaan Laboratorium </t>
   </si>
@@ -1060,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1244,6 +1244,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1261,12 +1270,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4971,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4997,13 +5000,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -5093,8 +5096,12 @@
       <c r="E18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
@@ -5104,7 +5111,8 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
@@ -5118,7 +5126,8 @@
       <c r="E20" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
@@ -5132,7 +5141,8 @@
       <c r="E21" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
@@ -5146,7 +5156,8 @@
       <c r="E22" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
@@ -5160,7 +5171,12 @@
       <c r="E23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="69">
+        <v>4</v>
+      </c>
+      <c r="G23" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
@@ -5174,7 +5190,12 @@
       <c r="E24" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="69">
+        <v>1</v>
+      </c>
+      <c r="G24" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
@@ -5188,7 +5209,12 @@
       <c r="E25" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="69">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
@@ -5202,7 +5228,12 @@
       <c r="E26" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="69">
+        <v>50</v>
+      </c>
+      <c r="G26" s="12">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
@@ -5216,7 +5247,12 @@
       <c r="E27" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="69">
+        <v>25</v>
+      </c>
+      <c r="G27" s="12">
+        <v>35</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
@@ -5230,7 +5266,12 @@
       <c r="E28" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="69">
+        <v>4</v>
+      </c>
+      <c r="G28" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
@@ -5244,7 +5285,12 @@
       <c r="E29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="69">
+        <v>1</v>
+      </c>
+      <c r="G29" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
@@ -5258,7 +5304,12 @@
       <c r="E30" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="69">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
@@ -5272,7 +5323,12 @@
       <c r="E31" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="69">
+        <v>4300000</v>
+      </c>
+      <c r="G31" s="12">
+        <v>5900000</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
@@ -5286,9 +5342,14 @@
       <c r="E32" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="69">
+        <v>13.4</v>
+      </c>
+      <c r="G32" s="12">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>29</v>
       </c>
@@ -5300,9 +5361,14 @@
       <c r="E33" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F33" s="69">
+        <v>45</v>
+      </c>
+      <c r="G33" s="12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>30</v>
       </c>
@@ -5314,9 +5380,14 @@
       <c r="E34" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F34" s="69">
+        <v>80</v>
+      </c>
+      <c r="G34" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>31</v>
       </c>
@@ -5328,9 +5399,14 @@
       <c r="E35" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F35" s="69">
+        <v>26</v>
+      </c>
+      <c r="G35" s="12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>32</v>
       </c>
@@ -5342,9 +5418,14 @@
       <c r="E36" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="69">
+        <v>31</v>
+      </c>
+      <c r="G36" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>33</v>
       </c>
@@ -5356,9 +5437,14 @@
       <c r="E37" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F37" s="69">
+        <v>10</v>
+      </c>
+      <c r="G37" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>34</v>
       </c>
@@ -5370,9 +5456,14 @@
       <c r="E38" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="69">
+        <v>37</v>
+      </c>
+      <c r="G38" s="12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>35</v>
       </c>
@@ -5384,9 +5475,14 @@
       <c r="E39" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F39" s="69">
+        <v>150000</v>
+      </c>
+      <c r="G39" s="12">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>36</v>
       </c>
@@ -5398,9 +5494,14 @@
       <c r="E40" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F40" s="69">
+        <v>7</v>
+      </c>
+      <c r="G40" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>37</v>
       </c>
@@ -5412,9 +5513,14 @@
       <c r="E41" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F41" s="69">
+        <v>10</v>
+      </c>
+      <c r="G41" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>38</v>
       </c>
@@ -5426,9 +5532,14 @@
       <c r="E42" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F42" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>39</v>
       </c>
@@ -5438,21 +5549,22 @@
       <c r="E43" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="69"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -5465,7 +5577,7 @@
       </c>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
@@ -5478,11 +5590,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -5538,13 +5650,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -5856,11 +5968,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -5915,13 +6027,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6199,11 +6311,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6258,13 +6370,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6534,11 +6646,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6593,13 +6705,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -6868,11 +6980,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -6928,13 +7040,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7235,11 +7347,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -7294,13 +7406,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7533,11 +7645,11 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="71" t="s">
+      <c r="B36" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
       <c r="E36" s="3" t="s">
         <v>72</v>
       </c>
@@ -7592,13 +7704,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -7881,11 +7993,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -7940,13 +8052,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8241,11 +8353,11 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="3" t="s">
         <v>72</v>
       </c>
@@ -8300,13 +8412,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8663,11 +8775,11 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="71" t="s">
+      <c r="B45" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="71"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="3" t="s">
         <v>72</v>
       </c>
@@ -8717,13 +8829,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -8802,12 +8914,12 @@
       <c r="A18" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
       <c r="F18" s="45"/>
       <c r="G18" s="26"/>
     </row>
@@ -8815,40 +8927,40 @@
       <c r="A19" s="61" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
         <v>255</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="2"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -9004,11 +9116,11 @@
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="71" t="s">
+      <c r="B43" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
       <c r="E43" s="3" t="s">
         <v>72</v>
       </c>
@@ -9037,8 +9149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9063,13 +9175,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -9159,10 +9271,10 @@
       <c r="E18" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="76" t="s">
+      <c r="F18" s="71" t="s">
         <v>267</v>
       </c>
-      <c r="G18" s="76" t="s">
+      <c r="G18" s="71" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9405,10 +9517,10 @@
       <c r="E32" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="75">
+      <c r="F32" s="70">
         <v>11.4</v>
       </c>
-      <c r="G32" s="75">
+      <c r="G32" s="70">
         <v>15.1</v>
       </c>
     </row>
@@ -9595,10 +9707,10 @@
       <c r="E42" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="75">
+      <c r="F42" s="70">
         <v>0.2</v>
       </c>
-      <c r="G42" s="75">
+      <c r="G42" s="70">
         <v>0.5</v>
       </c>
     </row>
@@ -9653,11 +9765,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -9785,13 +9897,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -10266,11 +10378,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -10325,13 +10437,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -10806,11 +10918,11 @@
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="3" t="s">
         <v>72</v>
       </c>
@@ -10865,13 +10977,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -11248,11 +11360,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -11302,13 +11414,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -11685,11 +11797,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -11739,13 +11851,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -12122,11 +12234,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -12176,13 +12288,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -12559,11 +12671,11 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="3" t="s">
         <v>72</v>
       </c>
@@ -12613,13 +12725,13 @@
       <c r="H6" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -13032,11 +13144,11 @@
       <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
+      <c r="C48" s="72"/>
+      <c r="D48" s="72"/>
       <c r="E48" s="3" t="s">
         <v>72</v>
       </c>

</xml_diff>